<commit_message>
licze x - xsr
</commit_message>
<xml_diff>
--- a/obliczenia.xlsx
+++ b/obliczenia.xlsx
@@ -331,7 +331,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B12"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -339,7 +339,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -347,8 +347,12 @@
         <f>A2^2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <f>A2-$A$12</f>
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -356,8 +360,12 @@
         <f t="shared" ref="B3:B11" si="0">A3^2</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <f t="shared" ref="C3:C11" si="1">A3-$A$12</f>
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -365,8 +373,12 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -374,8 +386,12 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -383,8 +399,12 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -392,8 +412,12 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -401,8 +425,12 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -410,8 +438,12 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -419,8 +451,12 @@
         <f t="shared" si="0"/>
         <v>81</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -428,8 +464,12 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>AVERAGE(A2:A11)</f>
         <v>5.5</v>
@@ -437,6 +477,10 @@
       <c r="B12">
         <f>AVERAGE(B2:B11)</f>
         <v>38.5</v>
+      </c>
+      <c r="C12">
+        <f>AVERAGE(C2:C11)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
podnosze do kwadratu moment
</commit_message>
<xml_diff>
--- a/obliczenia.xlsx
+++ b/obliczenia.xlsx
@@ -331,15 +331,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C12"/>
+  <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -351,8 +351,12 @@
         <f>A2-$A$12</f>
         <v>-4.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <f>C2^2</f>
+        <v>20.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -364,8 +368,12 @@
         <f t="shared" ref="C3:C11" si="1">A3-$A$12</f>
         <v>-3.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <f t="shared" ref="D3:D11" si="2">C3^2</f>
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -377,8 +385,12 @@
         <f t="shared" si="1"/>
         <v>-2.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -390,8 +402,12 @@
         <f t="shared" si="1"/>
         <v>-1.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -403,8 +419,12 @@
         <f t="shared" si="1"/>
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -416,8 +436,12 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -429,8 +453,12 @@
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -442,8 +470,12 @@
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -455,8 +487,12 @@
         <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -468,8 +504,12 @@
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>20.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>AVERAGE(A2:A11)</f>
         <v>5.5</v>
@@ -481,6 +521,10 @@
       <c r="C12">
         <f>AVERAGE(C2:C11)</f>
         <v>0</v>
+      </c>
+      <c r="D12">
+        <f>AVERAGE(D2:D11)</f>
+        <v>8.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>